<commit_message>
Update Conditional Format Table.xlsx
</commit_message>
<xml_diff>
--- a/Excel & Visual Basic/Examples/Conditional Format Table.xlsx
+++ b/Excel & Visual Basic/Examples/Conditional Format Table.xlsx
@@ -58479,8 +58479,8 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010028CAD5B0D39EEF4180FAF78645AB3BF3" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f49186227370304721ff655cee31aed">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e58ca87-4072-470e-8b31-171c5a2c0324" xmlns:ns3="a194edfb-0d26-4a04-9fce-796958ba02c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0965fcafb6e25e5ad89b6cd3a1350ad6" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010028CAD5B0D39EEF4180FAF78645AB3BF3" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe62ec5d3e4532085a00c0a90c3a20f3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e58ca87-4072-470e-8b31-171c5a2c0324" xmlns:ns3="a194edfb-0d26-4a04-9fce-796958ba02c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7878ea80cfe52bb681564f4bdb01e156" ns2:_="" ns3:_="">
     <xsd:import namespace="0e58ca87-4072-470e-8b31-171c5a2c0324"/>
     <xsd:import namespace="a194edfb-0d26-4a04-9fce-796958ba02c9"/>
     <xsd:element name="properties">
@@ -58496,6 +58496,10 @@
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -58531,6 +58535,28 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="15" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -58708,5 +58734,5 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4CF02FEE-79CD-432D-88A7-948C2E61050B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE88F882-CABC-4EF5-BC06-6DB5E052D4B6}"/>
 </file>
</xml_diff>